<commit_message>
change bom resistor footprint names
</commit_message>
<xml_diff>
--- a/hardware/IoT_color_detection_BOM.xlsx
+++ b/hardware/IoT_color_detection_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\altium_designer\color_detection\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDADF6E-D2D9-44DD-A30E-52E7EA12E8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6083AB50-0C6D-473D-BBB5-B938587A971B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C5C8E360-BF63-4451-B647-4E7148F02F12}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
   <si>
     <t>Comment</t>
   </si>
@@ -378,24 +378,6 @@
   </si>
   <si>
     <t>LED_Red</t>
-  </si>
-  <si>
-    <t>SMD_1207</t>
-  </si>
-  <si>
-    <t>SMD_1208</t>
-  </si>
-  <si>
-    <t>SMD_1209</t>
-  </si>
-  <si>
-    <t>SMD_1210</t>
-  </si>
-  <si>
-    <t>SMD_1211</t>
-  </si>
-  <si>
-    <t>SMD_1212</t>
   </si>
 </sst>
 </file>
@@ -510,16 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -529,6 +502,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -867,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E8ED98-220A-4EEA-8A05-1D06BB32283E}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,7 +879,7 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -906,7 +888,7 @@
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1</v>
       </c>
     </row>
@@ -914,14 +896,14 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1</v>
       </c>
     </row>
@@ -929,14 +911,14 @@
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1</v>
       </c>
     </row>
@@ -944,249 +926,249 @@
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="7">
         <v>1</v>
       </c>
     </row>
@@ -1194,7 +1176,7 @@
       <c r="A21" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1203,368 +1185,368 @@
       <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="8" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="8" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="7"/>
+      <c r="C30" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="10">
+      <c r="D30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="10">
+      <c r="D31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="10">
+      <c r="D32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E33" s="10">
+      <c r="D33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="10">
+      <c r="D34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D35" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="10">
+      <c r="D35" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E35" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="8" t="s">
+      <c r="B36" s="7"/>
+      <c r="C36" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="10">
+      <c r="E36" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="10"/>
-      <c r="C37" s="8" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="10">
+      <c r="E37" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="8" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E40" s="10">
+      <c r="E40" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E41" s="10">
+      <c r="E41" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="8" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="10">
+      <c r="E42" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="10"/>
-      <c r="C43" s="8" t="s">
+      <c r="B43" s="7"/>
+      <c r="C43" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="10"/>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>